<commit_message>
fix(data): fill Events.blockPolicy with valid default
Co-authored-by: hszqf <5326791+hszqf@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/GameData/Local/game_data.xlsx
+++ b/GameData/Local/game_data.xlsx
@@ -26862,8 +26862,6 @@
           <t>AN_001</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -26882,7 +26880,11 @@
           <t>收容单元内检测到时空扭曲，影响范围4.7平方米。需要紧急决策干预，已记录6份异常数据报告。</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -26896,7 +26898,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>0.15</v>
       </c>
@@ -26924,8 +26925,6 @@
           <t>AN_001</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -26944,7 +26943,11 @@
           <t>技术部门检测到维度门的异常指数指数下降至86%。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -26958,7 +26961,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
         <v>0.08</v>
       </c>
@@ -26986,8 +26988,6 @@
           <t>AN_002</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27006,7 +27006,11 @@
           <t>研究员报告周围4名D级人员出现生理异常症状。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27020,7 +27024,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
         <v>0.15</v>
       </c>
@@ -27048,8 +27051,6 @@
           <t>AN_002</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27068,7 +27069,11 @@
           <t>安保系统显示导致特斯拉防护网负荷达到96%。安保部门请求授权采取应急措施，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -27082,7 +27087,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>0.08</v>
       </c>
@@ -27110,8 +27114,6 @@
           <t>AN_003</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27130,7 +27132,11 @@
           <t>对AN_003进行的第35次观测中发现使7件标准设备出现功能异常。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27144,7 +27150,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
         <v>0.15</v>
       </c>
@@ -27172,8 +27177,6 @@
           <t>AN_004</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27192,7 +27195,11 @@
           <t>站点监测系统记录到失声合唱触发了2处独立监测点的警报。需要权衡资源投入与潜在风险。</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27206,7 +27213,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
         <v>0.15</v>
       </c>
@@ -27234,8 +27240,6 @@
           <t>AN_005</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27254,7 +27258,11 @@
           <t>收容单元内引发局部区域模因扩散，持续140秒。触发了应急预案，等待上级指示，已记录7份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27268,7 +27276,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>0.15</v>
       </c>
@@ -27296,8 +27303,6 @@
           <t>AN_005</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27316,7 +27321,11 @@
           <t>技术部门检测到AN_005的休谟上升82%，超出安全阈值。研究小组建议暂停当前收容流程。</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -27330,7 +27339,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
         <v>0.08</v>
       </c>
@@ -27358,8 +27366,6 @@
           <t>AN_006</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27378,7 +27384,11 @@
           <t>研究员报告造成收容区斯克兰顿现实稳定锚运行异常。站点主管需做出最终裁决，已记录10份异常数据报告。</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27392,7 +27402,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
         <v>0.15</v>
       </c>
@@ -27420,8 +27429,6 @@
           <t>AN_006</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27440,7 +27447,11 @@
           <t>安保系统显示产生2次异常能量波动，峰值91焦耳。收容协议要求立即响应，已记录12份异常数据报告。</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -27454,7 +27465,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>0.08</v>
       </c>
@@ -27482,8 +27492,6 @@
           <t>AN_007</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27502,7 +27510,11 @@
           <t>对AN_007进行的第41次观测中发现导致危险等级读数偏离正常值67个标准差。需要紧急决策干预。</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27516,7 +27528,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
         <v>0.15</v>
       </c>
@@ -27544,8 +27555,6 @@
           <t>AN_008</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27564,7 +27573,11 @@
           <t>站点监测系统记录到现实崩解出现8次信息辐射，持续时间37秒。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27578,7 +27591,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
         <v>0.15</v>
       </c>
@@ -27606,8 +27618,6 @@
           <t>AN_008</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27626,7 +27636,11 @@
           <t>收容单元内检测到概率场扰动，影响范围1.8平方米。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -27640,7 +27654,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>0.08</v>
       </c>
@@ -27668,8 +27681,6 @@
           <t>AN_009</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27688,7 +27699,11 @@
           <t>技术部门检测到末日预言的熵值指数上升至87%。安保部门请求授权采取应急措施，已记录8份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27702,7 +27717,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
         <v>0.15</v>
       </c>
@@ -27730,8 +27744,6 @@
           <t>AN_009</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27750,7 +27762,11 @@
           <t>研究员报告周围5名D级人员出现空间迷向症状。伦理委员会要求审核后续处理方案，已记录9份异常数据报告。</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -27764,7 +27780,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
         <v>0.08</v>
       </c>
@@ -27792,8 +27807,6 @@
           <t>AN_010</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27812,7 +27825,11 @@
           <t>安保系统显示导致负熵泵负荷达到96%。需要权衡资源投入与潜在风险，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27826,7 +27843,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
         <v>0.15</v>
       </c>
@@ -27854,8 +27870,6 @@
           <t>AN_011</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27874,7 +27888,11 @@
           <t>对AN_011进行的第47次观测中发现使4件标准设备出现功能异常。触发了应急预案，等待上级指示。</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -27888,7 +27906,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
         <v>0.15</v>
       </c>
@@ -27916,8 +27933,6 @@
           <t>AN_011</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27936,7 +27951,11 @@
           <t>站点监测系统记录到意识寄生触发了5处独立监测点的警报。研究小组建议暂停当前收容流程。</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -27950,7 +27969,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>0.08</v>
       </c>
@@ -27978,8 +27996,6 @@
           <t>AN_012</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -27998,7 +28014,11 @@
           <t>收容单元内引发局部区域因果紊乱，持续106秒。站点主管需做出最终裁决，已记录6份异常数据报告。</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28012,7 +28032,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>0.15</v>
       </c>
@@ -28040,8 +28059,6 @@
           <t>AN_013</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28060,7 +28077,11 @@
           <t>技术部门检测到形态模仿的扩散速度下降88%，超出安全阈值。收容协议要求立即响应。</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28074,7 +28095,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
         <v>0.15</v>
       </c>
@@ -28102,8 +28122,6 @@
           <t>AN_013</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28122,7 +28140,11 @@
           <t>研究员报告造成收容区Xyank时序调节器运行异常。需要紧急决策干预，已记录10份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -28136,7 +28158,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
         <v>0.08</v>
       </c>
@@ -28164,8 +28185,6 @@
           <t>AN_014</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28184,7 +28203,11 @@
           <t>安保系统显示产生5次异常能量波动，峰值90焦耳。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28198,7 +28221,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
         <v>0.15</v>
       </c>
@@ -28226,8 +28248,6 @@
           <t>AN_014</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28246,7 +28266,11 @@
           <t>对AN_014进行的第53次观测中发现导致现实稳定度读数偏离正常值74个标准差。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -28260,7 +28284,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
         <v>0.08</v>
       </c>
@@ -28288,8 +28311,6 @@
           <t>AN_015</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28308,7 +28329,11 @@
           <t>站点监测系统记录到静电蝴蝶出现4次时间流速异常，持续时间98秒。安保部门请求授权采取应急措施。</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J27" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28322,7 +28347,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr"/>
       <c r="N27" t="n">
         <v>0.15</v>
       </c>
@@ -28350,8 +28374,6 @@
           <t>AN_016</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28370,7 +28392,11 @@
           <t>收容单元内检测到空间折叠，影响范围7.7平方米。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J28" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28384,7 +28410,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
         <v>0.15</v>
       </c>
@@ -28412,8 +28437,6 @@
           <t>AN_017</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28432,7 +28455,11 @@
           <t>技术部门检测到虚空凝视的异常指数指数下降至92%。需要权衡资源投入与潜在风险，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J29" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28446,7 +28473,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr"/>
       <c r="N29" t="n">
         <v>0.15</v>
       </c>
@@ -28474,8 +28500,6 @@
           <t>AN_017</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28494,7 +28518,11 @@
           <t>研究员报告周围2名D级人员出现生理异常症状。触发了应急预案，等待上级指示，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -28508,7 +28536,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
         <v>0.08</v>
       </c>
@@ -28536,8 +28563,6 @@
           <t>AN_018</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28556,7 +28581,11 @@
           <t>安保系统显示导致休谟场发生器负荷达到88%。研究小组建议暂停当前收容流程，已记录10份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J31" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28570,7 +28599,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
         <v>0.15</v>
       </c>
@@ -28598,8 +28626,6 @@
           <t>AN_018</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28618,7 +28644,11 @@
           <t>对AN_018进行的第59次观测中发现使7件标准设备出现功能异常。站点主管需做出最终裁决。</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -28632,7 +28662,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
         <v>0.08</v>
       </c>
@@ -28660,8 +28689,6 @@
           <t>AN_019</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28680,7 +28707,11 @@
           <t>站点监测系统记录到共生幻影触发了3处独立监测点的警报。收容协议要求立即响应，已记录12份异常数据报告。</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28694,7 +28725,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
         <v>0.15</v>
       </c>
@@ -28722,8 +28752,6 @@
           <t>AN_019</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28742,7 +28770,11 @@
           <t>收容单元内引发局部区域时空扭曲，持续84秒。需要紧急决策干预，已记录9份异常数据报告。</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -28756,7 +28788,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
         <v>0.08</v>
       </c>
@@ -28784,8 +28815,6 @@
           <t>AN_020</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28804,7 +28833,11 @@
           <t>技术部门检测到梦境碎片的休谟上升73%，超出安全阈值。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J35" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28818,7 +28851,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
         <v>0.15</v>
       </c>
@@ -28846,8 +28878,6 @@
           <t>AN_021</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28866,7 +28896,11 @@
           <t>研究员报告造成收容区生物遏制单元运行异常。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J36" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -28880,7 +28914,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr"/>
       <c r="N36" t="n">
         <v>0.15</v>
       </c>
@@ -28908,8 +28941,6 @@
           <t>AN_021</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28928,7 +28959,11 @@
           <t>安保系统显示产生3次异常能量波动，峰值75焦耳。安保部门请求授权采取应急措施，已记录7份异常数据报告。</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J37" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -28942,7 +28977,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
         <v>0.08</v>
       </c>
@@ -28970,8 +29004,6 @@
           <t>AN_022</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -28990,7 +29022,11 @@
           <t>对AN_022进行的第65次观测中发现导致危险等级读数偏离正常值91个标准差。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J38" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29004,7 +29040,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M38" t="inlineStr"/>
       <c r="N38" t="n">
         <v>0.15</v>
       </c>
@@ -29032,8 +29067,6 @@
           <t>AN_023</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29052,7 +29085,11 @@
           <t>站点监测系统记录到影子玩偶出现3次认知污染，持续时间75秒。需要权衡资源投入与潜在风险。</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29066,7 +29103,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
         <v>0.15</v>
       </c>
@@ -29094,8 +29130,6 @@
           <t>AN_024</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29114,7 +29148,11 @@
           <t>收容单元内检测到模因扩散，影响范围7.3平方米。触发了应急预案，等待上级指示，已记录6份异常数据报告。</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29128,7 +29166,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
         <v>0.15</v>
       </c>
@@ -29156,8 +29193,6 @@
           <t>AN_024</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29176,7 +29211,11 @@
           <t>技术部门检测到思维回声的熵值指数下降至81%。研究小组建议暂停当前收容流程，已记录11份异常数据报告。</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J41" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -29190,7 +29229,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr"/>
       <c r="N41" t="n">
         <v>0.08</v>
       </c>
@@ -29218,8 +29256,6 @@
           <t>AN_025</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29238,7 +29274,11 @@
           <t>研究员报告周围4名D级人员出现空间迷向症状。站点主管需做出最终裁决，已记录8份异常数据报告。</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J42" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29252,7 +29292,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M42" t="inlineStr"/>
       <c r="N42" t="n">
         <v>0.15</v>
       </c>
@@ -29280,8 +29319,6 @@
           <t>AN_025</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29300,7 +29337,11 @@
           <t>安保系统显示导致特斯拉防护网负荷达到90%。收容协议要求立即响应，已记录7份异常数据报告。</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J43" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -29314,7 +29355,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M43" t="inlineStr"/>
       <c r="N43" t="n">
         <v>0.08</v>
       </c>
@@ -29342,8 +29382,6 @@
           <t>AN_026</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29362,7 +29400,11 @@
           <t>对AN_026进行的第71次观测中发现使3件标准设备出现功能异常。需要紧急决策干预。</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J44" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29376,7 +29418,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr"/>
       <c r="N44" t="n">
         <v>0.15</v>
       </c>
@@ -29404,8 +29445,6 @@
           <t>AN_026</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29424,7 +29463,11 @@
           <t>站点监测系统[已编辑]到无限增殖触发了4处独立监测点的警报。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J45" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -29438,7 +29481,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
         <v>0.08</v>
       </c>
@@ -29466,8 +29508,6 @@
           <t>AN_027</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29486,7 +29526,11 @@
           <t>收容单元内引发局部区域概率场扰动，持续61秒。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J46" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29500,7 +29544,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr"/>
       <c r="N46" t="n">
         <v>0.15</v>
       </c>
@@ -29528,8 +29571,6 @@
           <t>AN_027</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29548,7 +29589,11 @@
           <t>技术部门检测到预知镜面的扩散速度上升72%，超出安全阈值。安保部门请求授权采取应急措施。</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J47" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -29562,7 +29607,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M47" t="inlineStr"/>
       <c r="N47" t="n">
         <v>0.08</v>
       </c>
@@ -29590,8 +29634,6 @@
           <t>AN_028</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29610,7 +29652,11 @@
           <t>研究员报告造成收容区斯克兰顿现实稳定锚运行异常。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29624,7 +29670,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M48" t="inlineStr"/>
       <c r="N48" t="n">
         <v>0.15</v>
       </c>
@@ -29652,8 +29697,6 @@
           <t>AN_029</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29672,7 +29715,11 @@
           <t>安保系统显示产生8次异常能量波动，峰值70焦耳。需要权衡资源投入与潜在风险，已记录4份异常数据报告。</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29686,7 +29733,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr"/>
       <c r="N49" t="n">
         <v>0.15</v>
       </c>
@@ -29714,8 +29760,6 @@
           <t>AN_029</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29734,7 +29778,11 @@
           <t>对AN_029进行的第77次观测中发现导致现实稳定度读数偏离正常值79个标准差。触发了应急预案，等待上级指示。</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J50" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -29748,7 +29796,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr"/>
       <c r="N50" t="n">
         <v>0.08</v>
       </c>
@@ -29776,8 +29823,6 @@
           <t>AN_030</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29796,7 +29841,11 @@
           <t>站点监测系统记录到温度灯出现3次维度裂隙，持续时间57秒。研究小组建议暂停当前收容流程。</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J51" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29810,7 +29859,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr"/>
       <c r="N51" t="n">
         <v>0.15</v>
       </c>
@@ -29838,8 +29886,6 @@
           <t>AN_031</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29858,7 +29904,11 @@
           <t>收容单元内检测到因果紊乱，影响范围6.1平方米。站点主管需做出最终裁决，已记录11份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J52" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29872,7 +29922,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr"/>
       <c r="N52" t="n">
         <v>0.15</v>
       </c>
@@ -29900,8 +29949,6 @@
           <t>AN_031</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29920,7 +29967,11 @@
           <t>技术部门检测到时间吞噬的异常指数指数波动至72%。收容协议要求立即响应，已记录8份异常数据报告。</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J53" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -29934,7 +29985,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
         <v>0.08</v>
       </c>
@@ -29962,8 +30012,6 @@
           <t>AN_032</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -29982,7 +30030,11 @@
           <t>研究员报告周围2名D级人员出现生理异常症状。需要紧急决策干预，已记录11份异常数据报告。</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J54" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -29996,7 +30048,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M54" t="inlineStr"/>
       <c r="N54" t="n">
         <v>0.15</v>
       </c>
@@ -30024,8 +30075,6 @@
           <t>AN_033</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30044,7 +30093,11 @@
           <t>安保系统显示导致负熵泵负荷达到78%。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J55" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30058,7 +30111,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
         <v>0.15</v>
       </c>
@@ -30086,8 +30138,6 @@
           <t>AN_033</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30106,7 +30156,11 @@
           <t>对AN_033进行的第83次观测中发现使5件标准设备出现功能异常。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -30120,7 +30174,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr"/>
       <c r="N56" t="n">
         <v>0.08</v>
       </c>
@@ -30148,8 +30201,6 @@
           <t>AN_034</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30168,7 +30219,11 @@
           <t>站点监测系统记录到透明生物触发了3处独立监测点的警报。安保部门请求授权采取应急措施。</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30182,7 +30237,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr"/>
       <c r="N57" t="n">
         <v>0.15</v>
       </c>
@@ -30210,8 +30264,6 @@
           <t>AN_035</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30230,7 +30282,11 @@
           <t>收容单元内引发局部区域空间折叠，持续31秒。伦理委员会要求审核后续处理方案，已记录10份异常数据报告。</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J58" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30244,7 +30300,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr"/>
       <c r="N58" t="n">
         <v>0.15</v>
       </c>
@@ -30272,8 +30327,6 @@
           <t>AN_036</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30292,7 +30345,11 @@
           <t>技术部门检测到维度入侵的休谟波动95%，超出安全阈值。需要权衡资源投入与潜在风险。</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30306,7 +30363,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M59" t="inlineStr"/>
       <c r="N59" t="n">
         <v>0.15</v>
       </c>
@@ -30334,8 +30390,6 @@
           <t>AN_036</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30354,7 +30408,11 @@
           <t>研究员报告造成收容区Xyank时序调节器运行异常。触发了应急预案，等待上级指示。</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J60" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -30368,7 +30426,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M60" t="inlineStr"/>
       <c r="N60" t="n">
         <v>0.08</v>
       </c>
@@ -30396,8 +30453,6 @@
           <t>AN_037</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30416,7 +30471,11 @@
           <t>安保系统显示产生8次异常能量波动，峰值71焦耳。研究小组建议暂停当前收容流程，已记录3份异常数据报告。</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J61" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30430,7 +30489,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M61" t="inlineStr"/>
       <c r="N61" t="n">
         <v>0.15</v>
       </c>
@@ -30458,8 +30516,6 @@
           <t>AN_037</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30478,7 +30534,11 @@
           <t>对AN_037进行的第89次观测中发现导致危险等级读数偏离正常值84个标准差。站点主管需做出最终裁决。</t>
         </is>
       </c>
-      <c r="I62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J62" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -30492,7 +30552,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M62" t="inlineStr"/>
       <c r="N62" t="n">
         <v>0.08</v>
       </c>
@@ -30520,8 +30579,6 @@
           <t>AN_038</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30540,7 +30597,11 @@
           <t>站点监测系统记录到平行投影出现2次能量峰值，持续时间95秒。收容协议要求立即响应。</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J63" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30554,7 +30615,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M63" t="inlineStr"/>
       <c r="N63" t="n">
         <v>0.15</v>
       </c>
@@ -30582,8 +30642,6 @@
           <t>AN_038</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30602,7 +30660,11 @@
           <t>收容单元内检测到时空扭曲，影响范围4.6平方米。需要紧急决策干预，已记录4份异常数据报告。</t>
         </is>
       </c>
-      <c r="I64" t="inlineStr"/>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J64" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -30616,7 +30678,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M64" t="inlineStr"/>
       <c r="N64" t="n">
         <v>0.08</v>
       </c>
@@ -30644,8 +30705,6 @@
           <t>AN_039</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30664,7 +30723,11 @@
           <t>技术部门检测到AN_039的熵值指数上升至91%。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J65" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30678,7 +30741,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M65" t="inlineStr"/>
       <c r="N65" t="n">
         <v>0.15</v>
       </c>
@@ -30706,8 +30768,6 @@
           <t>AN_039</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30726,7 +30786,11 @@
           <t>研究员报告周围3名D级人员出现空间迷向症状。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J66" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -30740,7 +30804,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M66" t="inlineStr"/>
       <c r="N66" t="n">
         <v>0.08</v>
       </c>
@@ -30768,8 +30831,6 @@
           <t>AN_040</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30788,7 +30849,11 @@
           <t>安保系统显示导致休谟场发生器负荷达到86%。安保部门请求授权采取应急措施，已记录8份异常数据报告。</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr"/>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J67" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30802,7 +30867,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M67" t="inlineStr"/>
       <c r="N67" t="n">
         <v>0.15</v>
       </c>
@@ -30830,8 +30894,6 @@
           <t>AN_040</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30850,7 +30912,11 @@
           <t>对AN_040进行的第95次观测中发现使6件标准设备出现功能异常。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr"/>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J68" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -30864,7 +30930,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M68" t="inlineStr"/>
       <c r="N68" t="n">
         <v>0.08</v>
       </c>
@@ -30892,8 +30957,6 @@
           <t>AN_041</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30912,7 +30975,11 @@
           <t>站点监测系统记录到记忆书签触发了8处独立监测点的警报。需要权衡资源投入与潜在风险。</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr"/>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J69" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30926,7 +30993,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M69" t="inlineStr"/>
       <c r="N69" t="n">
         <v>0.15</v>
       </c>
@@ -30954,8 +31020,6 @@
           <t>AN_042</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -30974,7 +31038,11 @@
           <t>收容单元内引发局部区域模因扩散，持续118秒。触发了应急预案，等待上级指示，已记录6份异常数据报告。</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr"/>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J70" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -30988,7 +31056,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M70" t="inlineStr"/>
       <c r="N70" t="n">
         <v>0.15</v>
       </c>
@@ -31016,8 +31083,6 @@
           <t>AN_042</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31036,7 +31101,11 @@
           <t>技术部门检测到时空褶皱的扩散速度上升70%，超出安全阈值。研究小组建议暂停当前收容流程。</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr"/>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J71" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31050,7 +31119,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M71" t="inlineStr"/>
       <c r="N71" t="n">
         <v>0.08</v>
       </c>
@@ -31078,8 +31146,6 @@
           <t>AN_043</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31098,7 +31164,11 @@
           <t>研究员报告造成收容区生物遏制单元运行异常。站点主管需做出最终裁决，已记录7份异常数据报告。</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J72" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31112,7 +31182,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr"/>
       <c r="N72" t="n">
         <v>0.15</v>
       </c>
@@ -31140,8 +31209,6 @@
           <t>AN_043</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31160,7 +31227,11 @@
           <t>安保系统显示产生4次异常能量波动，峰值69焦耳。收容协议要求立即响应，已记录8份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr"/>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J73" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31174,7 +31245,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr"/>
       <c r="N73" t="n">
         <v>0.08</v>
       </c>
@@ -31202,8 +31272,6 @@
           <t>AN_044</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31222,7 +31290,11 @@
           <t>对AN_044进行的第101次观测中发现导致现实稳定度读数偏离正常值66个标准差。需要紧急决策干预。</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr"/>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J74" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31236,7 +31308,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr"/>
       <c r="N74" t="n">
         <v>0.15</v>
       </c>
@@ -31264,8 +31335,6 @@
           <t>AN_044</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31284,7 +31353,11 @@
           <t>站点监测系统记录到熵增加速出现6次信息辐射，持续时间80秒。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr"/>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J75" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31298,7 +31371,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M75" t="inlineStr"/>
       <c r="N75" t="n">
         <v>0.08</v>
       </c>
@@ -31326,8 +31398,6 @@
           <t>AN_045</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31346,7 +31416,11 @@
           <t>收容单元内检测到概率场扰动，影响范围7.2平方米。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr"/>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J76" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31360,7 +31434,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M76" t="inlineStr"/>
       <c r="N76" t="n">
         <v>0.15</v>
       </c>
@@ -31388,8 +31461,6 @@
           <t>AN_045</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31408,7 +31479,11 @@
           <t>技术部门检测到因果断裂的异常指数指数上升至65%。安保部门请求授权采取应急措施。</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr"/>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J77" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31422,7 +31497,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M77" t="inlineStr"/>
       <c r="N77" t="n">
         <v>0.08</v>
       </c>
@@ -31450,8 +31524,6 @@
           <t>AN_046</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31470,7 +31542,11 @@
           <t>研究员报告周围7名D级人员出现生理异常症状。伦理委员会要求审核后续处理方案，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I78" t="inlineStr"/>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J78" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31484,7 +31560,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M78" t="inlineStr"/>
       <c r="N78" t="n">
         <v>0.15</v>
       </c>
@@ -31512,8 +31587,6 @@
           <t>AN_046</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31532,7 +31605,11 @@
           <t>安保系统显示导致特斯拉防护网负荷达到98%。需要权衡资源投入与潜在风险，已记录9份异常数据报告。</t>
         </is>
       </c>
-      <c r="I79" t="inlineStr"/>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J79" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31546,7 +31623,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M79" t="inlineStr"/>
       <c r="N79" t="n">
         <v>0.08</v>
       </c>
@@ -31574,8 +31650,6 @@
           <t>AN_047</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31594,7 +31668,11 @@
           <t>对AN_047进行的第107次观测中发现使3件标准设备出现功能异常。触发了应急预案，等待上级指示。</t>
         </is>
       </c>
-      <c r="I80" t="inlineStr"/>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31608,7 +31686,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M80" t="inlineStr"/>
       <c r="N80" t="n">
         <v>0.15</v>
       </c>
@@ -31636,8 +31713,6 @@
           <t>AN_048</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31656,7 +31731,11 @@
           <t>站点监测系统记录到全知之眼触发了5处独立监测点的警报。研究小组建议暂停当前收容流程。</t>
         </is>
       </c>
-      <c r="I81" t="inlineStr"/>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J81" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31670,7 +31749,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M81" t="inlineStr"/>
       <c r="N81" t="n">
         <v>0.15</v>
       </c>
@@ -31698,8 +31776,6 @@
           <t>AN_048</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31718,7 +31794,11 @@
           <t>收容单元内引发局部区域因果紊乱，持续111秒。站点主管需做出最终裁决，已记录10份异常数据报告。</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr"/>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J82" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31732,7 +31812,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M82" t="inlineStr"/>
       <c r="N82" t="n">
         <v>0.08</v>
       </c>
@@ -31760,8 +31839,6 @@
           <t>AN_049</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31780,7 +31857,11 @@
           <t>技术部门检测到寒霜种子的休谟上升90%，超出安全阈值。收容协议要求立即响应，已记录7份异常数据报告。</t>
         </is>
       </c>
-      <c r="I83" t="inlineStr"/>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J83" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31794,7 +31875,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M83" t="inlineStr"/>
       <c r="N83" t="n">
         <v>0.15</v>
       </c>
@@ -31822,8 +31902,6 @@
           <t>AN_050</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31842,7 +31920,11 @@
           <t>研究员报告造成收容区斯克兰顿现实稳定锚运行异常。需要紧急决策干预，已记录11份异常数据报告。</t>
         </is>
       </c>
-      <c r="I84" t="inlineStr"/>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J84" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31856,7 +31938,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M84" t="inlineStr"/>
       <c r="N84" t="n">
         <v>0.15</v>
       </c>
@@ -31884,8 +31965,6 @@
           <t>AN_051</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31904,7 +31983,11 @@
           <t>安保系统显示产生7次异常能量波动，峰值90焦耳。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr"/>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J85" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -31918,7 +32001,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M85" t="inlineStr"/>
       <c r="N85" t="n">
         <v>0.15</v>
       </c>
@@ -31946,8 +32028,6 @@
           <t>AN_051</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -31966,7 +32046,11 @@
           <t>对AN_051进行的第113次观测中发现导致危险等级读数偏离正常值73个标准差。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J86" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -31980,7 +32064,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M86" t="inlineStr"/>
       <c r="N86" t="n">
         <v>0.08</v>
       </c>
@@ -32008,8 +32091,6 @@
           <t>AN_052</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32028,7 +32109,11 @@
           <t>站点监测系统[已编辑]到AN_052出现4次时间流速异常，持续时间94秒。安保部门请求授权采取应急措施。</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr"/>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J87" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32042,7 +32127,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M87" t="inlineStr"/>
       <c r="N87" t="n">
         <v>0.15</v>
       </c>
@@ -32070,8 +32154,6 @@
           <t>AN_052</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32090,7 +32172,11 @@
           <t>收容单元内检测到空间折叠，影响范围3.3平方米。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I88" t="inlineStr"/>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J88" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -32104,7 +32190,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M88" t="inlineStr"/>
       <c r="N88" t="n">
         <v>0.08</v>
       </c>
@@ -32132,8 +32217,6 @@
           <t>AN_053</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32152,7 +32235,11 @@
           <t>技术部门检测到记忆羽毛的熵值指数上升至73%。需要权衡资源投入与潜在风险，已记录12份异常数据报告。</t>
         </is>
       </c>
-      <c r="I89" t="inlineStr"/>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J89" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32166,7 +32253,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M89" t="inlineStr"/>
       <c r="N89" t="n">
         <v>0.15</v>
       </c>
@@ -32194,8 +32280,6 @@
           <t>AN_054</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32214,7 +32298,11 @@
           <t>研究员报告周围3名D级人员出现空间迷向症状。触发了应急预案，等待上级指示，已记录8份异常数据报告。</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr"/>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J90" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32228,7 +32316,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M90" t="inlineStr"/>
       <c r="N90" t="n">
         <v>0.15</v>
       </c>
@@ -32256,8 +32343,6 @@
           <t>AN_054</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32276,7 +32361,11 @@
           <t>安保系统显示导致负熵泵负荷达到88%。研究小组建议暂停当前收容流程，已记录8份异常数据报告。</t>
         </is>
       </c>
-      <c r="I91" t="inlineStr"/>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J91" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -32290,7 +32379,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M91" t="inlineStr"/>
       <c r="N91" t="n">
         <v>0.08</v>
       </c>
@@ -32318,8 +32406,6 @@
           <t>AN_055</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32338,7 +32424,11 @@
           <t>对AN_055进行的第119次观测中发现使3件标准设备出现功能异常。站点主管需做出最终裁决。</t>
         </is>
       </c>
-      <c r="I92" t="inlineStr"/>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J92" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32352,7 +32442,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M92" t="inlineStr"/>
       <c r="N92" t="n">
         <v>0.15</v>
       </c>
@@ -32380,8 +32469,6 @@
           <t>AN_055</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32400,7 +32487,11 @@
           <t>站点监测系统记录到熵之终结触发了4处独立监测点的警报。收容协议要求立即响应，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I93" t="inlineStr"/>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J93" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -32414,7 +32505,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M93" t="inlineStr"/>
       <c r="N93" t="n">
         <v>0.08</v>
       </c>
@@ -32442,8 +32532,6 @@
           <t>AN_056</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32462,7 +32550,11 @@
           <t>收容单元内引发局部区域时空扭曲，持续86秒。需要紧急决策干预，已记录10份异常[数据删除]报告。</t>
         </is>
       </c>
-      <c r="I94" t="inlineStr"/>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J94" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32476,7 +32568,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M94" t="inlineStr"/>
       <c r="N94" t="n">
         <v>0.15</v>
       </c>
@@ -32504,8 +32595,6 @@
           <t>AN_056</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32524,7 +32613,11 @@
           <t>技术部门检测到维度寄生的扩散速度下降85%，超出安全阈值。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I95" t="inlineStr"/>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J95" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -32538,7 +32631,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M95" t="inlineStr"/>
       <c r="N95" t="n">
         <v>0.08</v>
       </c>
@@ -32566,8 +32658,6 @@
           <t>AN_057</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32586,7 +32676,11 @@
           <t>研究员报告造成收容区Xyank时序调节器运行异常。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I96" t="inlineStr"/>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J96" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32600,7 +32694,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M96" t="inlineStr"/>
       <c r="N96" t="n">
         <v>0.15</v>
       </c>
@@ -32628,8 +32721,6 @@
           <t>AN_058</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32648,7 +32739,11 @@
           <t>安保系统显示产生4次异常能量波动，峰值73焦耳。安保部门请求授权采取应急措施，已记录4份异常数据报告。</t>
         </is>
       </c>
-      <c r="I97" t="inlineStr"/>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J97" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32662,7 +32757,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M97" t="inlineStr"/>
       <c r="N97" t="n">
         <v>0.15</v>
       </c>
@@ -32690,8 +32784,6 @@
           <t>AN_058</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32710,7 +32802,11 @@
           <t>对AN_058进行的第125次观测中发现导致现实稳定度读数偏离正常值83个标准差。伦理委员会要求审核后续处理方案。</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr"/>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J98" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -32724,7 +32820,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M98" t="inlineStr"/>
       <c r="N98" t="n">
         <v>0.08</v>
       </c>
@@ -32752,8 +32847,6 @@
           <t>AN_059</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32772,7 +32865,11 @@
           <t>站点监测系统记录到共鸣音叉出现5次认知污染，持续时间170秒。需要权衡资源投入与潜在风险。</t>
         </is>
       </c>
-      <c r="I99" t="inlineStr"/>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J99" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32786,7 +32883,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M99" t="inlineStr"/>
       <c r="N99" t="n">
         <v>0.15</v>
       </c>
@@ -32814,8 +32910,6 @@
           <t>AN_060</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32834,7 +32928,11 @@
           <t>收容单元内检测到模因扩散，影响范围7.9平方米。触发了应急预案，等待上级指示，已记录7份异常数据报告。</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr"/>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J100" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32848,7 +32946,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M100" t="inlineStr"/>
       <c r="N100" t="n">
         <v>0.15</v>
       </c>
@@ -32876,8 +32973,6 @@
           <t>AN_060</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32896,7 +32991,11 @@
           <t>技术部门检测到AN_060的异常指数指数波动至73%。研究小组建议暂停当前收容流程。</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr"/>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J101" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -32910,7 +33009,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M101" t="inlineStr"/>
       <c r="N101" t="n">
         <v>0.08</v>
       </c>
@@ -32938,8 +33036,6 @@
           <t>AN_061</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -32958,7 +33054,11 @@
           <t>研究员报告周围8名D级人员出现生理异常症状。站点主管需做出最终裁决，已记录5份异常数据报告。</t>
         </is>
       </c>
-      <c r="I102" t="inlineStr"/>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J102" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -32972,7 +33072,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M102" t="inlineStr"/>
       <c r="N102" t="n">
         <v>0.15</v>
       </c>
@@ -33000,8 +33099,6 @@
           <t>AN_062</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -33020,7 +33117,11 @@
           <t>安保系统显示导致休谟场发生器负荷达到96%。收容协议要求立即响应，已记录7份异常数据报告。</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr"/>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J103" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -33034,7 +33135,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M103" t="inlineStr"/>
       <c r="N103" t="n">
         <v>0.15</v>
       </c>
@@ -33062,8 +33162,6 @@
           <t>AN_063</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -33082,7 +33180,11 @@
           <t>对AN_063进行的第131次观测中发现使8件标准设备出现功能异常。需要紧急决策干预。</t>
         </is>
       </c>
-      <c r="I104" t="inlineStr"/>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J104" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -33096,7 +33198,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M104" t="inlineStr"/>
       <c r="N104" t="n">
         <v>0.15</v>
       </c>
@@ -33124,8 +33225,6 @@
           <t>AN_063</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -33144,7 +33243,11 @@
           <t>站点监测系统记录到信息黑洞触发了3处独立监测点的警报。技术部门提交了多套应对方案，需要主管裁决。</t>
         </is>
       </c>
-      <c r="I105" t="inlineStr"/>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J105" t="inlineStr">
         <is>
           <t>Global,OriginTask</t>
@@ -33158,7 +33261,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M105" t="inlineStr"/>
       <c r="N105" t="n">
         <v>0.08</v>
       </c>
@@ -33186,8 +33288,6 @@
           <t>AN_064</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -33206,7 +33306,11 @@
           <t>收容单元内引发局部区域概率场扰动，持续76秒。现有收容措施已接近临界值，要求调整策略。</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr"/>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J106" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -33220,7 +33324,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M106" t="inlineStr"/>
       <c r="N106" t="n">
         <v>0.15</v>
       </c>
@@ -33248,8 +33351,6 @@
           <t>AN_065</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr">
         <is>
           <t>RandomDaily</t>
@@ -33268,7 +33369,11 @@
           <t>技术部门检测到数字虫的休谟波动90%，超出安全阈值。安保部门请求授权采取应急措施。</t>
         </is>
       </c>
-      <c r="I107" t="inlineStr"/>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="J107" t="inlineStr">
         <is>
           <t>OriginTask</t>
@@ -33282,7 +33387,6 @@
           <t>ApplyDailyKeep</t>
         </is>
       </c>
-      <c r="M107" t="inlineStr"/>
       <c r="N107" t="n">
         <v>0.15</v>
       </c>

</xml_diff>

<commit_message>
feat(data): Add Excel tables for MediaProfiles, FactTemplates, FactTypes and MinNewsPerDay
- Added MinNewsPerDay to Balance table in Excel
- Created MediaProfiles table with FORMAL/SENSATIONAL/INVESTIGATIVE profiles
- Created FactTemplates table mapping fact types to profiles
- Created FactTypes table for fact type validation
- Updated DataRegistry to load new tables
- Modified FactNewsGenerator to read from registry with fallback
- Added EmitFact validation to warn on unknown fact types

Co-authored-by: hszqf <5326791+hszqf@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/GameData/Local/game_data.xlsx
+++ b/GameData/Local/game_data.xlsx
@@ -17,6 +17,9 @@
     <sheet name="EventOptions" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Effects" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="EffectOps" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="MediaProfiles" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="FactTemplates" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="FactTypes" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -16421,13 +16424,471 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>MediaProfiles</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>profileId</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>tone</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FORMAL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>正式报道</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SENSATIONAL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>耸人听闻</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>alarmist</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>INVESTIGATIVE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>调查报道</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>analytical</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>FactTemplates</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>templateId</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>factType</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>mediaProfileId</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>severityMin</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>severityMax</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>#comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>int</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FT_ANOMALY_FORMAL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AnomalySpawned</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>FORMAL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>异常生成-正式报道</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FT_ANOMALY_SENSATIONAL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AnomalySpawned</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SENSATIONAL</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>异常生成-耸人听闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FT_INV_COMPLETE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>InvestigateCompleted</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>INVESTIGATIVE</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>调查完成</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FT_INV_NORESULT</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>InvestigateNoResult</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>FORMAL</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>调查无果</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FT_CONTAIN_COMPLETE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ContainCompleted</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>FORMAL</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>收容完成</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>FactTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>typeId</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AnomalySpawned</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>异常生成事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>InvestigateCompleted</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>调查任务完成</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>InvestigateNoResult</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>调查任务无结果</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ContainCompleted</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>收容任务完成</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -16685,6 +17146,21 @@
       <c r="E15" s="2" t="inlineStr">
         <is>
           <t>Money 不允许负数：后续做日志提示更友好</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MinNewsPerDay</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>每日最少新闻数（用于Fact新闻不足时补充RandomDaily）</t>
         </is>
       </c>
     </row>

</xml_diff>